<commit_message>
Fixed problem from naming differences (Cav1 vs CaV1). Altered mRNAInfo to make updated the names easier.
</commit_message>
<xml_diff>
--- a/inst/extdata/mRNAInfo.xlsx
+++ b/inst/extdata/mRNAInfo.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Box Sync\AllWorkProjects\mRNA24hLC\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F09F73F7-E8A4-44B9-8227-BF999B5D9B0B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF69F5C-ED99-4DDD-9D00-782A5D7FF7F5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6740" yWindow="4210" windowWidth="21030" windowHeight="12970"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mRNAInfo" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="325">
   <si>
     <t>Table</t>
   </si>
@@ -947,12 +955,60 @@
   </si>
   <si>
     <t>mgabar3</t>
+  </si>
+  <si>
+    <t>InDataLower</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>kcnh1</t>
+  </si>
+  <si>
+    <t>cbnav</t>
+  </si>
+  <si>
+    <t>dar1a</t>
+  </si>
+  <si>
+    <t>dopa1br</t>
+  </si>
+  <si>
+    <t>dar2</t>
+  </si>
+  <si>
+    <t>x5htr1br</t>
+  </si>
+  <si>
+    <t>htr2</t>
+  </si>
+  <si>
+    <t>his1r</t>
+  </si>
+  <si>
+    <t>his2r</t>
+  </si>
+  <si>
+    <t>his3r</t>
+  </si>
+  <si>
+    <t>gababr1</t>
+  </si>
+  <si>
+    <t>mgaba2</t>
+  </si>
+  <si>
+    <t>mgaba3</t>
+  </si>
+  <si>
+    <t>lcch3r</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1794,24 +1850,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H102"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D59" sqref="D59"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L60" sqref="L60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="52.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1834,10 +1890,13 @@
         <v>287</v>
       </c>
       <c r="H1" t="s">
+        <v>309</v>
+      </c>
+      <c r="I1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1859,8 +1918,11 @@
       <c r="G2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1882,8 +1944,11 @@
       <c r="G3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1905,8 +1970,11 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1928,8 +1996,11 @@
       <c r="G5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1951,8 +2022,11 @@
       <c r="G6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1974,8 +2048,11 @@
       <c r="G7" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H7" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1997,8 +2074,11 @@
       <c r="G8" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2021,10 +2101,13 @@
         <v>288</v>
       </c>
       <c r="H9" t="s">
+        <v>311</v>
+      </c>
+      <c r="I9" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2046,8 +2129,11 @@
       <c r="G10" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2069,8 +2155,11 @@
       <c r="G11" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H11" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2092,8 +2181,11 @@
       <c r="G12" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H12" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2115,8 +2207,11 @@
       <c r="G13" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H13" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2138,8 +2233,11 @@
       <c r="G14" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H14" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2161,8 +2259,11 @@
       <c r="G15" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H15" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2184,8 +2285,11 @@
       <c r="G16" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H16" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2207,8 +2311,11 @@
       <c r="G17" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H17" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2230,8 +2337,11 @@
       <c r="G18" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H18" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2253,8 +2363,11 @@
       <c r="G19" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H19" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2276,8 +2389,11 @@
       <c r="G20" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H20" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2300,10 +2416,13 @@
         <v>215</v>
       </c>
       <c r="H21" t="s">
+        <v>312</v>
+      </c>
+      <c r="I21" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2</v>
       </c>
@@ -2325,8 +2444,11 @@
       <c r="G22" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H22" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2</v>
       </c>
@@ -2349,10 +2471,13 @@
         <v>291</v>
       </c>
       <c r="H23" t="s">
+        <v>291</v>
+      </c>
+      <c r="I23" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2</v>
       </c>
@@ -2374,8 +2499,11 @@
       <c r="G24" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H24" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2</v>
       </c>
@@ -2397,8 +2525,11 @@
       <c r="G25" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H25" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2</v>
       </c>
@@ -2420,8 +2551,11 @@
       <c r="G26" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H26" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2</v>
       </c>
@@ -2443,8 +2577,11 @@
       <c r="G27" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H27" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2</v>
       </c>
@@ -2467,10 +2604,13 @@
         <v>221</v>
       </c>
       <c r="H28" t="s">
+        <v>221</v>
+      </c>
+      <c r="I28" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2</v>
       </c>
@@ -2493,10 +2633,13 @@
         <v>222</v>
       </c>
       <c r="H29" t="s">
+        <v>222</v>
+      </c>
+      <c r="I29" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2</v>
       </c>
@@ -2519,10 +2662,13 @@
         <v>223</v>
       </c>
       <c r="H30" t="s">
+        <v>223</v>
+      </c>
+      <c r="I30" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2</v>
       </c>
@@ -2545,10 +2691,13 @@
         <v>224</v>
       </c>
       <c r="H31" t="s">
+        <v>224</v>
+      </c>
+      <c r="I31" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2</v>
       </c>
@@ -2571,10 +2720,13 @@
         <v>225</v>
       </c>
       <c r="H32" t="s">
+        <v>225</v>
+      </c>
+      <c r="I32" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2</v>
       </c>
@@ -2596,8 +2748,11 @@
       <c r="G33" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H33" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2</v>
       </c>
@@ -2619,8 +2774,11 @@
       <c r="G34" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H34" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2</v>
       </c>
@@ -2642,8 +2800,11 @@
       <c r="G35" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H35" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>3</v>
       </c>
@@ -2663,8 +2824,11 @@
       <c r="G36" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H36" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>3</v>
       </c>
@@ -2684,8 +2848,11 @@
       <c r="G37" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H37" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2705,8 +2872,11 @@
       <c r="G38" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H38" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2726,8 +2896,11 @@
       <c r="G39" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H39" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2747,8 +2920,11 @@
       <c r="G40" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H40" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>3</v>
       </c>
@@ -2768,8 +2944,11 @@
       <c r="G41" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H41" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2790,10 +2969,13 @@
         <v>235</v>
       </c>
       <c r="H42" t="s">
+        <v>313</v>
+      </c>
+      <c r="I42" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2814,10 +2996,13 @@
         <v>236</v>
       </c>
       <c r="H43" t="s">
+        <v>314</v>
+      </c>
+      <c r="I43" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2838,10 +3023,13 @@
         <v>237</v>
       </c>
       <c r="H44" t="s">
+        <v>315</v>
+      </c>
+      <c r="I44" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2861,8 +3049,11 @@
       <c r="G45" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H45" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2883,10 +3074,13 @@
         <v>239</v>
       </c>
       <c r="H46" t="s">
+        <v>316</v>
+      </c>
+      <c r="I46" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2907,10 +3101,13 @@
         <v>240</v>
       </c>
       <c r="H47" t="s">
+        <v>317</v>
+      </c>
+      <c r="I47" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2930,8 +3127,11 @@
       <c r="G48" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H48" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2952,10 +3152,13 @@
         <v>242</v>
       </c>
       <c r="H49" t="s">
+        <v>318</v>
+      </c>
+      <c r="I49" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2976,10 +3179,13 @@
         <v>243</v>
       </c>
       <c r="H50" t="s">
+        <v>319</v>
+      </c>
+      <c r="I50" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>3</v>
       </c>
@@ -3000,10 +3206,13 @@
         <v>244</v>
       </c>
       <c r="H51" t="s">
+        <v>320</v>
+      </c>
+      <c r="I51" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>3</v>
       </c>
@@ -3023,8 +3232,11 @@
       <c r="G52" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H52" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>3</v>
       </c>
@@ -3045,10 +3257,13 @@
         <v>246</v>
       </c>
       <c r="H53" t="s">
+        <v>321</v>
+      </c>
+      <c r="I53" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>3</v>
       </c>
@@ -3069,10 +3284,13 @@
         <v>247</v>
       </c>
       <c r="H54" t="s">
+        <v>322</v>
+      </c>
+      <c r="I54" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>299</v>
       </c>
@@ -3090,11 +3308,14 @@
       <c r="G55" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="H55" t="s">
+        <v>323</v>
+      </c>
+      <c r="I55" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>3</v>
       </c>
@@ -3115,10 +3336,13 @@
         <v>248</v>
       </c>
       <c r="H56" t="s">
+        <v>324</v>
+      </c>
+      <c r="I56" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>3</v>
       </c>
@@ -3138,8 +3362,11 @@
       <c r="G57" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H57" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>3</v>
       </c>
@@ -3159,8 +3386,11 @@
       <c r="G58" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H58" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>4</v>
       </c>
@@ -3179,8 +3409,11 @@
       <c r="G59" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H59" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>4</v>
       </c>
@@ -3199,8 +3432,11 @@
       <c r="G60" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H60" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>4</v>
       </c>
@@ -3219,8 +3455,11 @@
       <c r="G61" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H61" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>4</v>
       </c>
@@ -3239,8 +3478,11 @@
       <c r="G62" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H62" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>4</v>
       </c>
@@ -3259,8 +3501,11 @@
       <c r="G63" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H63" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>4</v>
       </c>
@@ -3279,8 +3524,11 @@
       <c r="G64" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H64" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>4</v>
       </c>
@@ -3300,10 +3548,13 @@
         <v>257</v>
       </c>
       <c r="H65" t="s">
+        <v>257</v>
+      </c>
+      <c r="I65" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>4</v>
       </c>
@@ -3323,10 +3574,13 @@
         <v>258</v>
       </c>
       <c r="H66" t="s">
+        <v>258</v>
+      </c>
+      <c r="I66" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>4</v>
       </c>
@@ -3346,10 +3600,13 @@
         <v>259</v>
       </c>
       <c r="H67" t="s">
+        <v>259</v>
+      </c>
+      <c r="I67" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>4</v>
       </c>
@@ -3369,10 +3626,13 @@
         <v>260</v>
       </c>
       <c r="H68" t="s">
+        <v>260</v>
+      </c>
+      <c r="I68" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>4</v>
       </c>
@@ -3392,10 +3652,13 @@
         <v>261</v>
       </c>
       <c r="H69" t="s">
+        <v>261</v>
+      </c>
+      <c r="I69" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>4</v>
       </c>
@@ -3415,10 +3678,13 @@
         <v>262</v>
       </c>
       <c r="H70" t="s">
+        <v>262</v>
+      </c>
+      <c r="I70" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>4</v>
       </c>
@@ -3438,10 +3704,13 @@
         <v>263</v>
       </c>
       <c r="H71" t="s">
+        <v>263</v>
+      </c>
+      <c r="I71" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>4</v>
       </c>
@@ -3461,10 +3730,13 @@
         <v>264</v>
       </c>
       <c r="H72" t="s">
+        <v>264</v>
+      </c>
+      <c r="I72" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>4</v>
       </c>
@@ -3484,10 +3756,13 @@
         <v>265</v>
       </c>
       <c r="H73" t="s">
+        <v>265</v>
+      </c>
+      <c r="I73" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>4</v>
       </c>
@@ -3507,10 +3782,13 @@
         <v>266</v>
       </c>
       <c r="H74" t="s">
+        <v>266</v>
+      </c>
+      <c r="I74" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>4</v>
       </c>
@@ -3530,10 +3808,13 @@
         <v>267</v>
       </c>
       <c r="H75" t="s">
+        <v>267</v>
+      </c>
+      <c r="I75" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>4</v>
       </c>
@@ -3553,10 +3834,13 @@
         <v>268</v>
       </c>
       <c r="H76" t="s">
+        <v>268</v>
+      </c>
+      <c r="I76" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>4</v>
       </c>
@@ -3576,10 +3860,13 @@
         <v>269</v>
       </c>
       <c r="H77" t="s">
+        <v>269</v>
+      </c>
+      <c r="I77" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>4</v>
       </c>
@@ -3598,8 +3885,11 @@
       <c r="G78" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H78" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>4</v>
       </c>
@@ -3618,8 +3908,11 @@
       <c r="G79" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H79" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>4</v>
       </c>
@@ -3638,8 +3931,11 @@
       <c r="G80" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H80" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>4</v>
       </c>
@@ -3658,8 +3954,11 @@
       <c r="G81" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H81" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>4</v>
       </c>
@@ -3678,8 +3977,11 @@
       <c r="G82" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H82" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>4</v>
       </c>
@@ -3698,8 +4000,11 @@
       <c r="G83" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H83" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>4</v>
       </c>
@@ -3718,8 +4023,11 @@
       <c r="G84" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H84" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>4</v>
       </c>
@@ -3738,8 +4046,11 @@
       <c r="G85" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H85" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>4</v>
       </c>
@@ -3758,8 +4069,11 @@
       <c r="G86" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H86" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>4</v>
       </c>
@@ -3778,8 +4092,11 @@
       <c r="G87" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H87" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>5</v>
       </c>
@@ -3798,8 +4115,11 @@
       <c r="G88" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H88" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>5</v>
       </c>
@@ -3818,8 +4138,11 @@
       <c r="G89" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H89" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>5</v>
       </c>
@@ -3838,8 +4161,11 @@
       <c r="G90" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H90" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>5</v>
       </c>
@@ -3858,8 +4184,11 @@
       <c r="G91" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H91" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>5</v>
       </c>
@@ -3878,8 +4207,11 @@
       <c r="G92" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H92" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>5</v>
       </c>
@@ -3898,8 +4230,11 @@
       <c r="G93" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H93" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>5</v>
       </c>
@@ -3918,8 +4253,11 @@
       <c r="G94" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H94" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>299</v>
       </c>
@@ -3939,11 +4277,14 @@
       <c r="G95" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="H95" s="1" t="s">
+      <c r="H95" t="s">
+        <v>290</v>
+      </c>
+      <c r="I95" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>299</v>
       </c>
@@ -3957,11 +4298,14 @@
       <c r="G96" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="H96" s="1" t="s">
+      <c r="H96" t="s">
+        <v>292</v>
+      </c>
+      <c r="I96" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>299</v>
       </c>
@@ -3975,11 +4319,14 @@
       <c r="G97" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="H97" s="1" t="s">
+      <c r="H97" t="s">
+        <v>294</v>
+      </c>
+      <c r="I97" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>299</v>
       </c>
@@ -3993,11 +4340,14 @@
       <c r="G98" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="H98" s="1" t="s">
+      <c r="H98" t="s">
+        <v>297</v>
+      </c>
+      <c r="I98" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>299</v>
       </c>
@@ -4011,11 +4361,14 @@
       <c r="G99" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="H99" s="1" t="s">
+      <c r="H99" t="s">
+        <v>298</v>
+      </c>
+      <c r="I99" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>299</v>
       </c>
@@ -4029,11 +4382,14 @@
       <c r="G100" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="H100" s="1" t="s">
+      <c r="H100" t="s">
+        <v>293</v>
+      </c>
+      <c r="I100" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>299</v>
       </c>
@@ -4047,11 +4403,14 @@
       <c r="G101" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="H101" s="1" t="s">
+      <c r="H101" t="s">
+        <v>295</v>
+      </c>
+      <c r="I101" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>299</v>
       </c>
@@ -4065,7 +4424,10 @@
       <c r="G102" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="H102" s="1" t="s">
+      <c r="H102" t="s">
+        <v>296</v>
+      </c>
+      <c r="I102" s="1" t="s">
         <v>177</v>
       </c>
     </row>

</xml_diff>